<commit_message>
add approximation for pictures ExposertimeOffset and added data to model
</commit_message>
<xml_diff>
--- a/ArtificalNeuronalColorNetwork/ANNServer/data.xlsx
+++ b/ArtificalNeuronalColorNetwork/ANNServer/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Documents\Arbeit\NewProjektFolder\Picture_Candela_Calculator\ArtificalNeuronalColorNetwork\ANNServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DC3D1A-2650-4404-9B5F-AD19B1826FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FA06DD-D74A-405E-AC77-FCE0A887C86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4130" yWindow="2240" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>rot</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>holz</t>
+  </si>
+  <si>
+    <t>farbkarte</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E208"/>
+  <dimension ref="A1:E250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="E256" sqref="E256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3307,6 +3310,597 @@
         <v>5</v>
       </c>
     </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>2.3701E-2</v>
+      </c>
+      <c r="B209">
+        <v>3.05659E-2</v>
+      </c>
+      <c r="C209">
+        <v>3.9891799999999998E-2</v>
+      </c>
+      <c r="D209" s="1">
+        <v>78</v>
+      </c>
+      <c r="E209" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>5.2868100000000001E-2</v>
+      </c>
+      <c r="B210">
+        <v>6.7843299999999995E-2</v>
+      </c>
+      <c r="C210">
+        <v>8.7756399999999998E-2</v>
+      </c>
+      <c r="D210" s="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>9.7904000000000005E-2</v>
+      </c>
+      <c r="B211">
+        <v>0.124985</v>
+      </c>
+      <c r="C211">
+        <v>0.16112599999999999</v>
+      </c>
+      <c r="D211" s="1">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>2.2047899999999999E-3</v>
+      </c>
+      <c r="B212">
+        <v>2.7542000000000001E-3</v>
+      </c>
+      <c r="C212">
+        <v>2.4131699999999999E-2</v>
+      </c>
+      <c r="D212" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>2.9576400000000001E-3</v>
+      </c>
+      <c r="B213">
+        <v>2.2209300000000001E-2</v>
+      </c>
+      <c r="C213">
+        <v>6.3851300000000001E-3</v>
+      </c>
+      <c r="D213" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>2.3538E-2</v>
+      </c>
+      <c r="B214">
+        <v>1.1210199999999999E-3</v>
+      </c>
+      <c r="C214">
+        <v>1.7938100000000001E-3</v>
+      </c>
+      <c r="D214" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>7.1219199999999996E-2</v>
+      </c>
+      <c r="B215">
+        <v>6.2068900000000003E-2</v>
+      </c>
+      <c r="C215">
+        <v>3.7238599999999998E-3</v>
+      </c>
+      <c r="D215" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>2.8636999999999999E-2</v>
+      </c>
+      <c r="B216">
+        <v>4.2324700000000003E-3</v>
+      </c>
+      <c r="C216">
+        <v>2.41303E-2</v>
+      </c>
+      <c r="D216" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>1.7621399999999999E-3</v>
+      </c>
+      <c r="B217">
+        <v>2.04779E-2</v>
+      </c>
+      <c r="C217">
+        <v>4.4483300000000003E-2</v>
+      </c>
+      <c r="D217" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>6.4635200000000004E-2</v>
+      </c>
+      <c r="B218">
+        <v>2.4043399999999999E-2</v>
+      </c>
+      <c r="C218">
+        <v>2.6160200000000002E-3</v>
+      </c>
+      <c r="D218" s="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>1.9385599999999999E-2</v>
+      </c>
+      <c r="B219">
+        <v>5.3315300000000003E-2</v>
+      </c>
+      <c r="C219">
+        <v>5.7833299999999997E-3</v>
+      </c>
+      <c r="D219" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>4.15498E-3</v>
+      </c>
+      <c r="B220">
+        <v>2.0171999999999998E-3</v>
+      </c>
+      <c r="C220">
+        <v>9.2993699999999995E-3</v>
+      </c>
+      <c r="D220" s="1">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>3.1255499999999999E-2</v>
+      </c>
+      <c r="B221">
+        <v>3.6996799999999999E-3</v>
+      </c>
+      <c r="C221">
+        <v>6.5318399999999997E-3</v>
+      </c>
+      <c r="D221" s="1">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>3.6369000000000002E-3</v>
+      </c>
+      <c r="B222">
+        <v>5.4739799999999998E-3</v>
+      </c>
+      <c r="C222">
+        <v>3.5549400000000002E-2</v>
+      </c>
+      <c r="D222" s="1">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>4.4679400000000001E-2</v>
+      </c>
+      <c r="B223">
+        <v>7.4349799999999999E-3</v>
+      </c>
+      <c r="C223">
+        <v>1.32923E-3</v>
+      </c>
+      <c r="D223" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>5.06544E-3</v>
+      </c>
+      <c r="B224">
+        <v>2.8142200000000001E-3</v>
+      </c>
+      <c r="C224">
+        <v>2.43706E-3</v>
+      </c>
+      <c r="D224" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A225">
+        <v>3.5876900000000003E-2</v>
+      </c>
+      <c r="B225">
+        <v>2.26079E-2</v>
+      </c>
+      <c r="C225">
+        <v>2.2552300000000001E-2</v>
+      </c>
+      <c r="D225" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226">
+        <v>5.6959799999999998E-3</v>
+      </c>
+      <c r="B226">
+        <v>1.2204E-2</v>
+      </c>
+      <c r="C226">
+        <v>3.34823E-2</v>
+      </c>
+      <c r="D226" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A227">
+        <v>2.9004299999999998E-3</v>
+      </c>
+      <c r="B227">
+        <v>5.6703500000000002E-3</v>
+      </c>
+      <c r="C227">
+        <v>2.6778399999999999E-3</v>
+      </c>
+      <c r="D227" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A228">
+        <v>1.30505E-2</v>
+      </c>
+      <c r="B228">
+        <v>1.4334899999999999E-2</v>
+      </c>
+      <c r="C228">
+        <v>4.88443E-2</v>
+      </c>
+      <c r="D228" s="1">
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A229">
+        <v>9.4468E-3</v>
+      </c>
+      <c r="B229">
+        <v>5.6413499999999998E-2</v>
+      </c>
+      <c r="C229">
+        <v>5.4308700000000001E-2</v>
+      </c>
+      <c r="D229" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A230">
+        <v>2.1636499999999999E-2</v>
+      </c>
+      <c r="B230">
+        <v>2.7144399999999999E-2</v>
+      </c>
+      <c r="C230">
+        <v>3.4917499999999997E-2</v>
+      </c>
+      <c r="D230" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A231">
+        <v>4.84266E-2</v>
+      </c>
+      <c r="B231">
+        <v>6.0453399999999997E-2</v>
+      </c>
+      <c r="C231">
+        <v>7.7494599999999997E-2</v>
+      </c>
+      <c r="D231" s="1">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A232">
+        <v>9.2013399999999995E-2</v>
+      </c>
+      <c r="B232">
+        <v>0.114135</v>
+      </c>
+      <c r="C232">
+        <v>0.14504500000000001</v>
+      </c>
+      <c r="D232" s="1">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A233">
+        <v>2.1565500000000001E-3</v>
+      </c>
+      <c r="B233">
+        <v>2.4702000000000001E-3</v>
+      </c>
+      <c r="C233">
+        <v>2.19087E-2</v>
+      </c>
+      <c r="D233" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A234">
+        <v>2.8321100000000001E-3</v>
+      </c>
+      <c r="B234">
+        <v>1.9775500000000001E-2</v>
+      </c>
+      <c r="C234">
+        <v>5.6569200000000002E-3</v>
+      </c>
+      <c r="D234" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A235">
+        <v>2.1475299999999999E-2</v>
+      </c>
+      <c r="B235">
+        <v>1.0560599999999999E-3</v>
+      </c>
+      <c r="C235">
+        <v>1.7290199999999999E-3</v>
+      </c>
+      <c r="D235" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A236">
+        <v>6.72566E-2</v>
+      </c>
+      <c r="B236">
+        <v>5.6219999999999999E-2</v>
+      </c>
+      <c r="C236">
+        <v>3.4998099999999999E-3</v>
+      </c>
+      <c r="D236" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A237">
+        <v>2.6381700000000001E-2</v>
+      </c>
+      <c r="B237">
+        <v>3.9327199999999998E-3</v>
+      </c>
+      <c r="C237">
+        <v>2.15371E-2</v>
+      </c>
+      <c r="D237" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A238">
+        <v>1.7120499999999999E-3</v>
+      </c>
+      <c r="B238">
+        <v>1.8289699999999999E-2</v>
+      </c>
+      <c r="C238">
+        <v>3.9763600000000003E-2</v>
+      </c>
+      <c r="D238" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A239">
+        <v>5.8779499999999998E-2</v>
+      </c>
+      <c r="B239">
+        <v>2.2137400000000002E-2</v>
+      </c>
+      <c r="C239">
+        <v>2.3088000000000002E-3</v>
+      </c>
+      <c r="D239" s="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A240">
+        <v>1.8159999999999999E-2</v>
+      </c>
+      <c r="B240">
+        <v>4.7862599999999998E-2</v>
+      </c>
+      <c r="C240">
+        <v>5.4136200000000001E-3</v>
+      </c>
+      <c r="D240" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A241">
+        <v>3.7201299999999999E-3</v>
+      </c>
+      <c r="B241">
+        <v>1.93721E-3</v>
+      </c>
+      <c r="C241">
+        <v>8.22758E-3</v>
+      </c>
+      <c r="D241" s="1">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A242">
+        <v>2.8906600000000001E-2</v>
+      </c>
+      <c r="B242">
+        <v>3.4510000000000001E-3</v>
+      </c>
+      <c r="C242">
+        <v>5.8234100000000002E-3</v>
+      </c>
+      <c r="D242" s="1">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A243">
+        <v>3.3527600000000002E-3</v>
+      </c>
+      <c r="B243">
+        <v>4.9668999999999998E-3</v>
+      </c>
+      <c r="C243">
+        <v>3.1616900000000003E-2</v>
+      </c>
+      <c r="D243" s="1">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A244">
+        <v>4.1082599999999997E-2</v>
+      </c>
+      <c r="B244">
+        <v>6.8660500000000003E-3</v>
+      </c>
+      <c r="C244">
+        <v>1.2752900000000001E-3</v>
+      </c>
+      <c r="D244" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A245">
+        <v>4.7777499999999999E-3</v>
+      </c>
+      <c r="B245">
+        <v>2.6144900000000001E-3</v>
+      </c>
+      <c r="C245">
+        <v>2.3516399999999999E-3</v>
+      </c>
+      <c r="D245" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A246">
+        <v>3.2911700000000002E-2</v>
+      </c>
+      <c r="B246">
+        <v>2.0512699999999998E-2</v>
+      </c>
+      <c r="C246">
+        <v>2.0257899999999999E-2</v>
+      </c>
+      <c r="D246" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A247">
+        <v>5.1622899999999999E-3</v>
+      </c>
+      <c r="B247">
+        <v>1.10262E-2</v>
+      </c>
+      <c r="C247">
+        <v>2.9814500000000001E-2</v>
+      </c>
+      <c r="D247" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A248">
+        <v>2.7393500000000002E-3</v>
+      </c>
+      <c r="B248">
+        <v>5.3840700000000003E-3</v>
+      </c>
+      <c r="C248">
+        <v>2.48511E-3</v>
+      </c>
+      <c r="D248" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A249">
+        <v>1.1668400000000001E-2</v>
+      </c>
+      <c r="B249">
+        <v>1.29295E-2</v>
+      </c>
+      <c r="C249">
+        <v>4.3041299999999998E-2</v>
+      </c>
+      <c r="D249" s="1">
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A250">
+        <v>8.73203E-3</v>
+      </c>
+      <c r="B250">
+        <v>5.06454E-2</v>
+      </c>
+      <c r="C250">
+        <v>4.8091700000000001E-2</v>
+      </c>
+      <c r="D250" s="1">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
readme and data update
</commit_message>
<xml_diff>
--- a/ArtificalNeuronalColorNetwork/ANNServer/data.xlsx
+++ b/ArtificalNeuronalColorNetwork/ANNServer/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Documents\Arbeit\NewProjektFolder\Picture_Candela_Calculator\ArtificalNeuronalColorNetwork\ANNServer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\AppData\Local\Programs\Python\Python39\Lib\site-packages\ANNServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FA06DD-D74A-405E-AC77-FCE0A887C86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520FB976-8CED-4BF0-BABF-043724846FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4130" yWindow="2240" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1970" yWindow="3710" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:E235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="E256" sqref="E256"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,481 +937,484 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>7.3252999999999999E-3</v>
+        <v>1.38531E-2</v>
       </c>
       <c r="B40">
-        <v>8.0490200000000005E-3</v>
+        <v>1.4790899999999999E-2</v>
       </c>
       <c r="C40">
-        <v>1.18186E-2</v>
+        <v>2.2709900000000002E-2</v>
       </c>
       <c r="D40">
-        <v>50.6</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>1.38531E-2</v>
+        <v>2.6606899999999999E-2</v>
       </c>
       <c r="B41">
-        <v>1.4790899999999999E-2</v>
+        <v>2.8158300000000001E-2</v>
       </c>
       <c r="C41">
-        <v>2.2709900000000002E-2</v>
+        <v>4.4830700000000001E-2</v>
       </c>
       <c r="D41">
-        <v>76.8</v>
+        <v>113.6</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>2.6606899999999999E-2</v>
+        <v>4.4201299999999999E-2</v>
       </c>
       <c r="B42">
-        <v>2.8158300000000001E-2</v>
+        <v>4.5248999999999998E-2</v>
       </c>
       <c r="C42">
-        <v>4.4830700000000001E-2</v>
+        <v>7.27574E-2</v>
       </c>
       <c r="D42">
-        <v>113.6</v>
+        <v>152.80000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>4.4201299999999999E-2</v>
+        <v>7.57636E-2</v>
       </c>
       <c r="B43">
-        <v>4.5248999999999998E-2</v>
+        <v>7.7028399999999997E-2</v>
       </c>
       <c r="C43">
-        <v>7.27574E-2</v>
+        <v>0.118534</v>
       </c>
       <c r="D43">
-        <v>152.80000000000001</v>
+        <v>208.8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>7.57636E-2</v>
+        <v>0.11265</v>
       </c>
       <c r="B44">
-        <v>7.7028399999999997E-2</v>
+        <v>0.112674</v>
       </c>
       <c r="C44">
-        <v>0.118534</v>
+        <v>0.17930299999999999</v>
       </c>
       <c r="D44">
-        <v>208.8</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>0.11265</v>
+        <v>2.7214100000000001E-2</v>
       </c>
       <c r="B45">
-        <v>0.112674</v>
+        <v>2.8531899999999999E-2</v>
       </c>
       <c r="C45">
-        <v>0.17930299999999999</v>
+        <v>4.91131E-2</v>
       </c>
       <c r="D45">
-        <v>265</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>2.7214100000000001E-2</v>
+        <v>3.6301899999999998E-2</v>
       </c>
       <c r="B46">
-        <v>2.8531899999999999E-2</v>
+        <v>3.8305199999999998E-2</v>
       </c>
       <c r="C46">
-        <v>4.91131E-2</v>
+        <v>6.4562400000000006E-2</v>
       </c>
       <c r="D46">
-        <v>126</v>
+        <v>142.4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>3.6301899999999998E-2</v>
+        <v>3.9652600000000003E-2</v>
       </c>
       <c r="B47">
-        <v>3.8305199999999998E-2</v>
+        <v>4.1804599999999997E-2</v>
       </c>
       <c r="C47">
-        <v>6.4562400000000006E-2</v>
+        <v>6.9302100000000005E-2</v>
       </c>
       <c r="D47">
-        <v>142.4</v>
+        <v>148.19999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>3.9652600000000003E-2</v>
+        <v>4.7211500000000003E-2</v>
       </c>
       <c r="B48">
-        <v>4.1804599999999997E-2</v>
+        <v>4.8695500000000003E-2</v>
       </c>
       <c r="C48">
-        <v>6.9302100000000005E-2</v>
+        <v>8.1272700000000003E-2</v>
       </c>
       <c r="D48">
-        <v>148.19999999999999</v>
+        <v>162.30000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>4.7211500000000003E-2</v>
+        <v>5.9207599999999999E-2</v>
       </c>
       <c r="B49">
-        <v>4.8695500000000003E-2</v>
+        <v>6.2516600000000005E-2</v>
       </c>
       <c r="C49">
-        <v>8.1272700000000003E-2</v>
+        <v>9.83594E-2</v>
       </c>
       <c r="D49">
-        <v>162.30000000000001</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>5.9207599999999999E-2</v>
+        <v>6.8281900000000006E-2</v>
       </c>
       <c r="B50">
-        <v>6.2516600000000005E-2</v>
+        <v>7.1924600000000005E-2</v>
       </c>
       <c r="C50">
-        <v>9.83594E-2</v>
+        <v>0.11257499999999999</v>
       </c>
       <c r="D50">
-        <v>184</v>
+        <v>199.3</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>6.8281900000000006E-2</v>
+        <v>8.6195300000000002E-2</v>
       </c>
       <c r="B51">
-        <v>7.1924600000000005E-2</v>
+        <v>8.96729E-2</v>
       </c>
       <c r="C51">
-        <v>0.11257499999999999</v>
+        <v>0.13819100000000001</v>
       </c>
       <c r="D51">
-        <v>199.3</v>
+        <v>227.6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>8.6195300000000002E-2</v>
+        <v>0.1086</v>
       </c>
       <c r="B52">
-        <v>8.96729E-2</v>
+        <v>0.112002</v>
       </c>
       <c r="C52">
-        <v>0.13819100000000001</v>
+        <v>0.17716299999999999</v>
       </c>
       <c r="D52">
-        <v>227.6</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>0.1086</v>
+        <v>0.130803</v>
       </c>
       <c r="B53">
-        <v>0.112002</v>
+        <v>0.134021</v>
       </c>
       <c r="C53">
-        <v>0.17716299999999999</v>
+        <v>0.212924</v>
       </c>
       <c r="D53">
-        <v>262.5</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>0.130803</v>
+        <v>0.12889200000000001</v>
       </c>
       <c r="B54">
-        <v>0.134021</v>
+        <v>0.132961</v>
       </c>
       <c r="C54">
-        <v>0.212924</v>
+        <v>0.20916299999999999</v>
       </c>
       <c r="D54">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>0.12889200000000001</v>
+        <v>0.123282</v>
       </c>
       <c r="B55">
-        <v>0.132961</v>
+        <v>0.12299499999999999</v>
       </c>
       <c r="C55">
-        <v>0.20916299999999999</v>
+        <v>0.19700500000000001</v>
       </c>
       <c r="D55">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>0.123282</v>
+        <v>1.2919E-2</v>
       </c>
       <c r="B56">
-        <v>0.12299499999999999</v>
+        <v>1.3680100000000001E-2</v>
       </c>
       <c r="C56">
-        <v>0.19700500000000001</v>
+        <v>2.0502099999999999E-2</v>
       </c>
       <c r="D56">
-        <v>272</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>1.2919E-2</v>
+        <v>2.4943199999999999E-2</v>
       </c>
       <c r="B57">
-        <v>1.3680100000000001E-2</v>
+        <v>2.57691E-2</v>
       </c>
       <c r="C57">
-        <v>2.0502099999999999E-2</v>
+        <v>3.8848800000000003E-2</v>
       </c>
       <c r="D57">
-        <v>76.8</v>
+        <v>113.6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>2.4943199999999999E-2</v>
+        <v>4.1445999999999997E-2</v>
       </c>
       <c r="B58">
-        <v>2.57691E-2</v>
+        <v>4.1379399999999997E-2</v>
       </c>
       <c r="C58">
-        <v>3.8848800000000003E-2</v>
+        <v>6.2911400000000006E-2</v>
       </c>
       <c r="D58">
-        <v>113.6</v>
+        <v>152.80000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>4.1445999999999997E-2</v>
+        <v>7.2402999999999995E-2</v>
       </c>
       <c r="B59">
-        <v>4.1379399999999997E-2</v>
+        <v>7.1354600000000004E-2</v>
       </c>
       <c r="C59">
-        <v>6.2911400000000006E-2</v>
+        <v>0.102809</v>
       </c>
       <c r="D59">
-        <v>152.80000000000001</v>
+        <v>208.8</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>7.2402999999999995E-2</v>
+        <v>0.108983</v>
       </c>
       <c r="B60">
-        <v>7.1354600000000004E-2</v>
+        <v>0.10437</v>
       </c>
       <c r="C60">
-        <v>0.102809</v>
+        <v>0.15190300000000001</v>
       </c>
       <c r="D60">
-        <v>208.8</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>0.108983</v>
+        <v>2.6437499999999999E-2</v>
       </c>
       <c r="B61">
-        <v>0.10437</v>
+        <v>2.6376799999999999E-2</v>
       </c>
       <c r="C61">
-        <v>0.15190300000000001</v>
+        <v>3.9756699999999999E-2</v>
       </c>
       <c r="D61">
-        <v>265</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>2.6437499999999999E-2</v>
+        <v>3.45537E-2</v>
       </c>
       <c r="B62">
-        <v>2.6376799999999999E-2</v>
+        <v>3.4305000000000002E-2</v>
       </c>
       <c r="C62">
-        <v>3.9756699999999999E-2</v>
+        <v>5.1889600000000001E-2</v>
       </c>
       <c r="D62">
-        <v>126</v>
+        <v>142.4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>3.45537E-2</v>
+        <v>3.7779500000000001E-2</v>
       </c>
       <c r="B63">
-        <v>3.4305000000000002E-2</v>
+        <v>3.7175199999999999E-2</v>
       </c>
       <c r="C63">
-        <v>5.1889600000000001E-2</v>
+        <v>5.7234500000000001E-2</v>
       </c>
       <c r="D63">
-        <v>142.4</v>
+        <v>148.19999999999999</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>3.7779500000000001E-2</v>
+        <v>4.4519900000000001E-2</v>
       </c>
       <c r="B64">
-        <v>3.7175199999999999E-2</v>
+        <v>4.4143700000000001E-2</v>
       </c>
       <c r="C64">
-        <v>5.7234500000000001E-2</v>
+        <v>6.7386299999999996E-2</v>
       </c>
       <c r="D64">
-        <v>148.19999999999999</v>
+        <v>162.30000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>4.4519900000000001E-2</v>
+        <v>5.6983100000000002E-2</v>
       </c>
       <c r="B65">
-        <v>4.4143700000000001E-2</v>
+        <v>5.7023600000000001E-2</v>
       </c>
       <c r="C65">
-        <v>6.7386299999999996E-2</v>
+        <v>8.50355E-2</v>
       </c>
       <c r="D65">
-        <v>162.30000000000001</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>5.6983100000000002E-2</v>
+        <v>6.6316700000000006E-2</v>
       </c>
       <c r="B66">
-        <v>5.7023600000000001E-2</v>
+        <v>6.6691100000000003E-2</v>
       </c>
       <c r="C66">
-        <v>8.50355E-2</v>
+        <v>9.76186E-2</v>
       </c>
       <c r="D66">
-        <v>184</v>
+        <v>199.3</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>6.6316700000000006E-2</v>
+        <v>8.3787600000000004E-2</v>
       </c>
       <c r="B67">
-        <v>6.6691100000000003E-2</v>
+        <v>8.2565700000000006E-2</v>
       </c>
       <c r="C67">
-        <v>9.76186E-2</v>
+        <v>0.119181</v>
       </c>
       <c r="D67">
-        <v>199.3</v>
+        <v>227.6</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>8.3787600000000004E-2</v>
+        <v>0.106</v>
       </c>
       <c r="B68">
-        <v>8.2565700000000006E-2</v>
+        <v>0.102565</v>
       </c>
       <c r="C68">
-        <v>0.119181</v>
+        <v>0.15495300000000001</v>
       </c>
       <c r="D68">
-        <v>227.6</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>0.106</v>
+        <v>0.127632</v>
       </c>
       <c r="B69">
-        <v>0.102565</v>
+        <v>0.12404900000000001</v>
       </c>
       <c r="C69">
-        <v>0.15495300000000001</v>
+        <v>0.18182599999999999</v>
       </c>
       <c r="D69">
-        <v>262.5</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>0.127632</v>
+        <v>0.126836</v>
       </c>
       <c r="B70">
-        <v>0.12404900000000001</v>
+        <v>0.123486</v>
       </c>
       <c r="C70">
-        <v>0.18182599999999999</v>
+        <v>0.182391</v>
       </c>
       <c r="D70">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>0.126836</v>
+        <v>0.11755599999999999</v>
       </c>
       <c r="B71">
-        <v>0.123486</v>
+        <v>0.114035</v>
       </c>
       <c r="C71">
-        <v>0.182391</v>
+        <v>0.164463</v>
       </c>
       <c r="D71">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>0.11755599999999999</v>
+        <v>0.69735899999999995</v>
       </c>
       <c r="B72">
-        <v>0.114035</v>
+        <v>0.77867900000000001</v>
       </c>
       <c r="C72">
-        <v>0.164463</v>
-      </c>
-      <c r="D72">
-        <v>272</v>
+        <v>0.815944</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1770</v>
+      </c>
+      <c r="E72" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>0.69735899999999995</v>
+        <v>8.5971199999999998E-3</v>
       </c>
       <c r="B73">
-        <v>0.77867900000000001</v>
+        <v>4.8982499999999998E-3</v>
       </c>
       <c r="C73">
-        <v>0.815944</v>
+        <v>2.3341799999999999E-3</v>
       </c>
       <c r="D73" s="1">
-        <v>1770</v>
+        <v>52</v>
       </c>
       <c r="E73" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -1570,41 +1573,41 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>7.1391499999999997E-2</v>
+        <v>0.66147900000000004</v>
       </c>
       <c r="B85">
-        <v>0.154722</v>
+        <v>0.77166000000000001</v>
       </c>
       <c r="C85">
-        <v>0.88804499999999997</v>
+        <v>0.82017600000000002</v>
       </c>
       <c r="D85" s="1">
-        <v>147</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>0.66147900000000004</v>
+        <v>0.74441199999999996</v>
       </c>
       <c r="B86">
-        <v>0.77166000000000001</v>
+        <v>0.83838100000000004</v>
       </c>
       <c r="C86">
-        <v>0.82017600000000002</v>
+        <v>2.00194E-2</v>
       </c>
       <c r="D86" s="1">
-        <v>1600</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>0.74441199999999996</v>
+        <v>0.49937999999999999</v>
       </c>
       <c r="B87">
-        <v>0.83838100000000004</v>
+        <v>0.81067100000000003</v>
       </c>
       <c r="C87">
-        <v>2.00194E-2</v>
+        <v>0.83871700000000005</v>
       </c>
       <c r="D87" s="1">
         <v>1625</v>
@@ -1612,55 +1615,55 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>0.49937999999999999</v>
+        <v>0.32153700000000002</v>
       </c>
       <c r="B88">
-        <v>0.81067100000000003</v>
+        <v>0.88861199999999996</v>
       </c>
       <c r="C88">
-        <v>0.83871700000000005</v>
+        <v>0.13535900000000001</v>
       </c>
       <c r="D88" s="1">
-        <v>1625</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>0.32153700000000002</v>
+        <v>0.67731200000000003</v>
       </c>
       <c r="B89">
-        <v>0.88861199999999996</v>
+        <v>0.22753999999999999</v>
       </c>
       <c r="C89">
-        <v>0.13535900000000001</v>
+        <v>0.99936599999999998</v>
       </c>
       <c r="D89" s="1">
-        <v>1490</v>
+        <v>459</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>0.67731200000000003</v>
+        <v>0.675095</v>
       </c>
       <c r="B90">
-        <v>0.22753999999999999</v>
+        <v>0.77680800000000005</v>
       </c>
       <c r="C90">
-        <v>0.99936599999999998</v>
+        <v>7.1402000000000002E-3</v>
       </c>
       <c r="D90" s="1">
-        <v>459</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>0.675095</v>
+        <v>0.43130400000000002</v>
       </c>
       <c r="B91">
-        <v>0.77680800000000005</v>
+        <v>0.786304</v>
       </c>
       <c r="C91">
-        <v>7.1402000000000002E-3</v>
+        <v>0.80101199999999995</v>
       </c>
       <c r="D91" s="1">
         <v>1625</v>
@@ -1668,433 +1671,433 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>0.43130400000000002</v>
+        <v>0.29927999999999999</v>
       </c>
       <c r="B92">
-        <v>0.786304</v>
+        <v>0.87963999999999998</v>
       </c>
       <c r="C92">
-        <v>0.80101199999999995</v>
+        <v>0.10187599999999999</v>
       </c>
       <c r="D92" s="1">
-        <v>1625</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>0.29927999999999999</v>
+        <v>0.64037699999999997</v>
       </c>
       <c r="B93">
-        <v>0.87963999999999998</v>
+        <v>0.18504200000000001</v>
       </c>
       <c r="C93">
-        <v>0.10187599999999999</v>
+        <v>0.99943499999999996</v>
       </c>
       <c r="D93" s="1">
-        <v>1490</v>
+        <v>459</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>0.64037699999999997</v>
+        <v>0.64224599999999998</v>
       </c>
       <c r="B94">
-        <v>0.18504200000000001</v>
+        <v>9.3191200000000002E-3</v>
       </c>
       <c r="C94">
-        <v>0.99943499999999996</v>
+        <v>4.8083800000000001E-3</v>
       </c>
       <c r="D94" s="1">
-        <v>459</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
-        <v>0.64224599999999998</v>
+        <v>0.49493799999999999</v>
       </c>
       <c r="B95">
-        <v>9.3191200000000002E-3</v>
+        <v>0.507633</v>
       </c>
       <c r="C95">
-        <v>4.8083800000000001E-3</v>
+        <v>0.54113800000000001</v>
       </c>
       <c r="D95" s="1">
-        <v>275</v>
+        <v>985</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
-        <v>6.0827899999999997E-2</v>
+        <v>0.51327400000000001</v>
       </c>
       <c r="B96">
-        <v>0.11835</v>
+        <v>0.53568199999999999</v>
       </c>
       <c r="C96">
-        <v>0.86273500000000003</v>
+        <v>0.116734</v>
       </c>
       <c r="D96" s="1">
-        <v>147</v>
+        <v>980</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
-        <v>0.49493799999999999</v>
+        <v>0.35593900000000001</v>
       </c>
       <c r="B97">
-        <v>0.507633</v>
+        <v>0.61276799999999998</v>
       </c>
       <c r="C97">
-        <v>0.54113800000000001</v>
+        <v>0.63326499999999997</v>
       </c>
       <c r="D97" s="1">
-        <v>985</v>
+        <v>980</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
-        <v>0.51327400000000001</v>
+        <v>0.31917600000000002</v>
       </c>
       <c r="B98">
-        <v>0.53568199999999999</v>
+        <v>0.60321599999999997</v>
       </c>
       <c r="C98">
-        <v>0.116734</v>
+        <v>0.156975</v>
       </c>
       <c r="D98" s="1">
-        <v>980</v>
+        <v>933</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
-        <v>0.35593900000000001</v>
+        <v>0.48580099999999998</v>
       </c>
       <c r="B99">
-        <v>0.61276799999999998</v>
+        <v>0.24213799999999999</v>
       </c>
       <c r="C99">
-        <v>0.63326499999999997</v>
+        <v>0.69218900000000005</v>
       </c>
       <c r="D99" s="1">
-        <v>980</v>
+        <v>518</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
-        <v>0.31917600000000002</v>
+        <v>0.484429</v>
       </c>
       <c r="B100">
-        <v>0.60321599999999997</v>
+        <v>0.155528</v>
       </c>
       <c r="C100">
-        <v>0.156975</v>
+        <v>0.146374</v>
       </c>
       <c r="D100" s="1">
-        <v>933</v>
+        <v>460</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
-        <v>0.48580099999999998</v>
+        <v>0.249442</v>
       </c>
       <c r="B101">
-        <v>0.24213799999999999</v>
+        <v>0.21773500000000001</v>
       </c>
       <c r="C101">
-        <v>0.69218900000000005</v>
+        <v>0.61934999999999996</v>
       </c>
       <c r="D101" s="1">
-        <v>518</v>
+        <v>383</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
-        <v>0.484429</v>
+        <v>0.31672600000000001</v>
       </c>
       <c r="B102">
-        <v>0.155528</v>
+        <v>0.40293099999999998</v>
       </c>
       <c r="C102">
-        <v>0.146374</v>
+        <v>0.464725</v>
       </c>
       <c r="D102" s="1">
-        <v>460</v>
+        <v>683</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
-        <v>0.249442</v>
+        <v>0.34223100000000001</v>
       </c>
       <c r="B103">
-        <v>0.21773500000000001</v>
+        <v>0.41700799999999999</v>
       </c>
       <c r="C103">
-        <v>0.61934999999999996</v>
+        <v>6.6617300000000003E-3</v>
       </c>
       <c r="D103" s="1">
-        <v>383</v>
+        <v>675</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
-        <v>0.31672600000000001</v>
+        <v>0.14310200000000001</v>
       </c>
       <c r="B104">
-        <v>0.40293099999999998</v>
+        <v>0.489674</v>
       </c>
       <c r="C104">
-        <v>0.464725</v>
+        <v>0.55346499999999998</v>
       </c>
       <c r="D104" s="1">
-        <v>683</v>
+        <v>675</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
-        <v>0.34223100000000001</v>
+        <v>9.7622700000000007E-2</v>
       </c>
       <c r="B105">
-        <v>0.41700799999999999</v>
+        <v>0.50116799999999995</v>
       </c>
       <c r="C105">
-        <v>6.6617300000000003E-3</v>
+        <v>2.1503299999999999E-2</v>
       </c>
       <c r="D105" s="1">
-        <v>675</v>
+        <v>630</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
-        <v>0.14310200000000001</v>
+        <v>0.293047</v>
       </c>
       <c r="B106">
-        <v>0.489674</v>
+        <v>7.34601E-2</v>
       </c>
       <c r="C106">
-        <v>0.55346499999999998</v>
+        <v>0.616622</v>
       </c>
       <c r="D106" s="1">
-        <v>675</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
-        <v>9.7622700000000007E-2</v>
+        <v>0.11669499999999999</v>
       </c>
       <c r="B107">
-        <v>0.50116799999999995</v>
+        <v>0.42091600000000001</v>
       </c>
       <c r="C107">
-        <v>2.1503299999999999E-2</v>
+        <v>0.465615</v>
       </c>
       <c r="D107" s="1">
-        <v>630</v>
+        <v>675</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
-        <v>0.293047</v>
+        <v>8.4218199999999993E-2</v>
       </c>
       <c r="B108">
-        <v>7.34601E-2</v>
+        <v>0.449596</v>
       </c>
       <c r="C108">
-        <v>0.616622</v>
+        <v>1.41753E-2</v>
       </c>
       <c r="D108" s="1">
-        <v>216</v>
+        <v>630</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
-        <v>0.11669499999999999</v>
+        <v>0.25689600000000001</v>
       </c>
       <c r="B109">
-        <v>0.42091600000000001</v>
+        <v>6.0672900000000002E-2</v>
       </c>
       <c r="C109">
-        <v>0.465615</v>
+        <v>0.57691999999999999</v>
       </c>
       <c r="D109" s="1">
-        <v>675</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
-        <v>8.4218199999999993E-2</v>
+        <v>0.21314</v>
       </c>
       <c r="B110">
-        <v>0.449596</v>
+        <v>7.4714600000000001E-3</v>
       </c>
       <c r="C110">
-        <v>1.41753E-2</v>
+        <v>6.0891000000000001E-3</v>
       </c>
       <c r="D110" s="1">
-        <v>630</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
-        <v>0.25689600000000001</v>
+        <v>2.51925E-2</v>
       </c>
       <c r="B111">
-        <v>6.0672900000000002E-2</v>
+        <v>4.0512199999999998E-2</v>
       </c>
       <c r="C111">
-        <v>0.57691999999999999</v>
+        <v>0.47377599999999997</v>
       </c>
       <c r="D111" s="1">
-        <v>216</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
-        <v>0.21314</v>
+        <v>0.30376700000000001</v>
       </c>
       <c r="B112">
-        <v>7.4714600000000001E-3</v>
+        <v>0.37912800000000002</v>
       </c>
       <c r="C112">
-        <v>6.0891000000000001E-3</v>
+        <v>0.43107899999999999</v>
       </c>
       <c r="D112" s="1">
-        <v>143</v>
+        <v>683</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
-        <v>2.51925E-2</v>
+        <v>0.33379599999999998</v>
       </c>
       <c r="B113">
-        <v>4.0512199999999998E-2</v>
+        <v>0.40271299999999999</v>
       </c>
       <c r="C113">
-        <v>0.47377599999999997</v>
+        <v>5.43949E-3</v>
       </c>
       <c r="D113" s="1">
-        <v>90</v>
+        <v>675</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
-        <v>0.30376700000000001</v>
+        <v>0.14106299999999999</v>
       </c>
       <c r="B114">
-        <v>0.37912800000000002</v>
+        <v>0.48314099999999999</v>
       </c>
       <c r="C114">
-        <v>0.43107899999999999</v>
+        <v>0.54873300000000003</v>
       </c>
       <c r="D114" s="1">
-        <v>683</v>
+        <v>675</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
-        <v>0.33379599999999998</v>
+        <v>9.7103999999999996E-2</v>
       </c>
       <c r="B115">
-        <v>0.40271299999999999</v>
+        <v>0.51335799999999998</v>
       </c>
       <c r="C115">
-        <v>5.43949E-3</v>
+        <v>2.2859999999999998E-2</v>
       </c>
       <c r="D115" s="1">
-        <v>675</v>
+        <v>630</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
-        <v>0.14106299999999999</v>
+        <v>0.31449899999999997</v>
       </c>
       <c r="B116">
-        <v>0.48314099999999999</v>
+        <v>7.9338099999999995E-2</v>
       </c>
       <c r="C116">
-        <v>0.54873300000000003</v>
+        <v>0.65707400000000005</v>
       </c>
       <c r="D116" s="1">
-        <v>675</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
-        <v>9.7103999999999996E-2</v>
+        <v>0.26826800000000001</v>
       </c>
       <c r="B117">
-        <v>0.51335799999999998</v>
+        <v>7.8023199999999997E-3</v>
       </c>
       <c r="C117">
-        <v>2.2859999999999998E-2</v>
+        <v>5.9712799999999998E-3</v>
       </c>
       <c r="D117" s="1">
-        <v>630</v>
+        <v>143</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
-        <v>0.31449899999999997</v>
+        <v>2.7326099999999999E-2</v>
       </c>
       <c r="B118">
-        <v>7.9338099999999995E-2</v>
+        <v>5.1789799999999997E-2</v>
       </c>
       <c r="C118">
-        <v>0.65707400000000005</v>
+        <v>0.523285</v>
       </c>
       <c r="D118" s="1">
-        <v>216</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
-        <v>0.26826800000000001</v>
+        <v>0.36458800000000002</v>
       </c>
       <c r="B119">
-        <v>7.8023199999999997E-3</v>
+        <v>0.364145</v>
       </c>
       <c r="C119">
-        <v>5.9712799999999998E-3</v>
+        <v>0.38321300000000003</v>
       </c>
       <c r="D119" s="1">
-        <v>143</v>
+        <v>670</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
-        <v>2.7326099999999999E-2</v>
+        <v>0.376946</v>
       </c>
       <c r="B120">
-        <v>5.1789799999999997E-2</v>
+        <v>0.37082700000000002</v>
       </c>
       <c r="C120">
-        <v>0.523285</v>
+        <v>0.13458100000000001</v>
       </c>
       <c r="D120" s="1">
-        <v>90</v>
+        <v>670</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
-        <v>0.36458800000000002</v>
+        <v>0.27706700000000001</v>
       </c>
       <c r="B121">
-        <v>0.364145</v>
+        <v>0.40624900000000003</v>
       </c>
       <c r="C121">
-        <v>0.38321300000000003</v>
+        <v>0.42122199999999999</v>
       </c>
       <c r="D121" s="1">
-        <v>670</v>
+        <v>690</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
-        <v>0.376946</v>
+        <v>0.36949900000000002</v>
       </c>
       <c r="B122">
-        <v>0.37082700000000002</v>
+        <v>0.344578</v>
       </c>
       <c r="C122">
-        <v>0.13458100000000001</v>
+        <v>0.12218900000000001</v>
       </c>
       <c r="D122" s="1">
         <v>670</v>
@@ -2102,13 +2105,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123">
-        <v>0.27706700000000001</v>
+        <v>0.283858</v>
       </c>
       <c r="B123">
-        <v>0.40624900000000003</v>
+        <v>0.41562100000000002</v>
       </c>
       <c r="C123">
-        <v>0.42122199999999999</v>
+        <v>0.444052</v>
       </c>
       <c r="D123" s="1">
         <v>690</v>
@@ -2116,1788 +2119,1575 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124">
-        <v>0.36949900000000002</v>
+        <v>0.26589600000000002</v>
       </c>
       <c r="B124">
-        <v>0.344578</v>
+        <v>0.39965000000000001</v>
       </c>
       <c r="C124">
-        <v>0.12218900000000001</v>
+        <v>0.14279</v>
       </c>
       <c r="D124" s="1">
-        <v>670</v>
+        <v>662</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
-        <v>0.283858</v>
+        <v>0.37482799999999999</v>
       </c>
       <c r="B125">
-        <v>0.41562100000000002</v>
+        <v>0.205979</v>
       </c>
       <c r="C125">
-        <v>0.444052</v>
+        <v>0.48670799999999997</v>
       </c>
       <c r="D125" s="1">
-        <v>690</v>
+        <v>465</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
-        <v>0.26589600000000002</v>
+        <v>0.35590500000000003</v>
       </c>
       <c r="B126">
-        <v>0.39965000000000001</v>
+        <v>0.146672</v>
       </c>
       <c r="C126">
-        <v>0.14279</v>
+        <v>0.14000399999999999</v>
       </c>
       <c r="D126" s="1">
-        <v>662</v>
+        <v>430</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
-        <v>0.37482799999999999</v>
+        <v>0.26212400000000002</v>
       </c>
       <c r="B127">
-        <v>0.205979</v>
+        <v>0.39143</v>
       </c>
       <c r="C127">
-        <v>0.48670799999999997</v>
+        <v>0.124638</v>
       </c>
       <c r="D127" s="1">
-        <v>465</v>
+        <v>662</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
-        <v>0.35590500000000003</v>
+        <v>0.38144299999999998</v>
       </c>
       <c r="B128">
-        <v>0.146672</v>
+        <v>0.20763499999999999</v>
       </c>
       <c r="C128">
-        <v>0.14000399999999999</v>
+        <v>0.49360300000000001</v>
       </c>
       <c r="D128" s="1">
-        <v>430</v>
+        <v>465</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129">
-        <v>0.26212400000000002</v>
+        <v>0.38374200000000003</v>
       </c>
       <c r="B129">
-        <v>0.39143</v>
+        <v>0.16400300000000001</v>
       </c>
       <c r="C129">
-        <v>0.124638</v>
+        <v>0.15743799999999999</v>
       </c>
       <c r="D129" s="1">
-        <v>662</v>
+        <v>430</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130">
-        <v>0.38144299999999998</v>
+        <v>0.26013500000000001</v>
       </c>
       <c r="B130">
-        <v>0.20763499999999999</v>
+        <v>0.209981</v>
       </c>
       <c r="C130">
-        <v>0.49360300000000001</v>
+        <v>0.454484</v>
       </c>
       <c r="D130" s="1">
-        <v>465</v>
+        <v>410</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131">
-        <v>0.38374200000000003</v>
+        <v>0.58623800000000004</v>
       </c>
       <c r="B131">
-        <v>0.16400300000000001</v>
+        <v>0.665072</v>
       </c>
       <c r="C131">
-        <v>0.15743799999999999</v>
-      </c>
-      <c r="D131" s="1">
-        <v>430</v>
+        <v>0.71930799999999995</v>
+      </c>
+      <c r="D131">
+        <v>1300</v>
+      </c>
+      <c r="E131">
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132">
-        <v>0.26013500000000001</v>
+        <v>0.62022999999999995</v>
       </c>
       <c r="B132">
-        <v>0.209981</v>
+        <v>0.67854199999999998</v>
       </c>
       <c r="C132">
-        <v>0.454484</v>
-      </c>
-      <c r="D132" s="1">
-        <v>410</v>
+        <v>6.8068699999999996E-2</v>
+      </c>
+      <c r="D132">
+        <v>1300</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133">
-        <v>0.58623800000000004</v>
+        <v>0.40272999999999998</v>
       </c>
       <c r="B133">
-        <v>0.665072</v>
+        <v>0.72806599999999999</v>
       </c>
       <c r="C133">
-        <v>0.71930799999999995</v>
+        <v>0.76846000000000003</v>
       </c>
       <c r="D133">
-        <v>1300</v>
-      </c>
-      <c r="E133">
-        <v>4</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134">
-        <v>0.62022999999999995</v>
+        <v>0.325069</v>
       </c>
       <c r="B134">
-        <v>0.67854199999999998</v>
+        <v>0.74741599999999997</v>
       </c>
       <c r="C134">
-        <v>6.8068699999999996E-2</v>
+        <v>0.14260700000000001</v>
       </c>
       <c r="D134">
-        <v>1300</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135">
-        <v>0.40272999999999998</v>
+        <v>0.56348500000000001</v>
       </c>
       <c r="B135">
-        <v>0.72806599999999999</v>
+        <v>0.23824500000000001</v>
       </c>
       <c r="C135">
-        <v>0.76846000000000003</v>
+        <v>0.87575499999999995</v>
       </c>
       <c r="D135">
-        <v>1270</v>
+        <v>522</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136">
-        <v>0.325069</v>
+        <v>0.56129499999999999</v>
       </c>
       <c r="B136">
-        <v>0.74741599999999997</v>
+        <v>0.62989600000000001</v>
       </c>
       <c r="C136">
-        <v>0.14260700000000001</v>
+        <v>0.67035100000000003</v>
       </c>
       <c r="D136">
-        <v>1215</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137">
-        <v>0.56348500000000001</v>
+        <v>0.60596499999999998</v>
       </c>
       <c r="B137">
-        <v>0.23824500000000001</v>
+        <v>0.66253700000000004</v>
       </c>
       <c r="C137">
-        <v>0.87575499999999995</v>
+        <v>5.7910999999999997E-2</v>
       </c>
       <c r="D137">
-        <v>522</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138">
-        <v>0.56129499999999999</v>
+        <v>0.39843899999999999</v>
       </c>
       <c r="B138">
-        <v>0.62989600000000001</v>
+        <v>0.72502299999999997</v>
       </c>
       <c r="C138">
-        <v>0.67035100000000003</v>
+        <v>0.75606300000000004</v>
       </c>
       <c r="D138">
-        <v>1300</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139">
-        <v>0.60596499999999998</v>
+        <v>0.329316</v>
       </c>
       <c r="B139">
-        <v>0.66253700000000004</v>
+        <v>0.76720699999999997</v>
       </c>
       <c r="C139">
-        <v>5.7910999999999997E-2</v>
+        <v>0.15083299999999999</v>
       </c>
       <c r="D139">
-        <v>1300</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140">
-        <v>0.39843899999999999</v>
+        <v>0.57453600000000005</v>
       </c>
       <c r="B140">
-        <v>0.72502299999999997</v>
+        <v>0.24457599999999999</v>
       </c>
       <c r="C140">
-        <v>0.75606300000000004</v>
+        <v>0.89362799999999998</v>
       </c>
       <c r="D140">
-        <v>1270</v>
+        <v>522</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141">
-        <v>0.329316</v>
+        <v>0.57616999999999996</v>
       </c>
       <c r="B141">
-        <v>0.76720699999999997</v>
+        <v>8.2320400000000002E-2</v>
       </c>
       <c r="C141">
-        <v>0.15083299999999999</v>
+        <v>6.5622700000000006E-2</v>
       </c>
       <c r="D141">
-        <v>1215</v>
+        <v>386</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142">
-        <v>0.57453600000000005</v>
+        <v>0.175204</v>
       </c>
       <c r="B142">
-        <v>0.24457599999999999</v>
+        <v>0.20039199999999999</v>
       </c>
       <c r="C142">
-        <v>0.89362799999999998</v>
+        <v>0.78714600000000001</v>
       </c>
       <c r="D142">
-        <v>522</v>
+        <v>315</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143">
-        <v>0.57616999999999996</v>
+        <v>0.53983599999999998</v>
       </c>
       <c r="B143">
-        <v>8.2320400000000002E-2</v>
+        <v>0.58663699999999996</v>
       </c>
       <c r="C143">
-        <v>6.5622700000000006E-2</v>
+        <v>4.4966100000000002E-2</v>
       </c>
       <c r="D143">
-        <v>386</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144">
-        <v>0.175204</v>
+        <v>0.352771</v>
       </c>
       <c r="B144">
-        <v>0.20039199999999999</v>
+        <v>0.67614300000000005</v>
       </c>
       <c r="C144">
-        <v>0.78714600000000001</v>
+        <v>0.69501599999999997</v>
       </c>
       <c r="D144">
-        <v>315</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145">
-        <v>0.53983599999999998</v>
+        <v>0.30952099999999999</v>
       </c>
       <c r="B145">
-        <v>0.58663699999999996</v>
+        <v>0.71531999999999996</v>
       </c>
       <c r="C145">
-        <v>4.4966100000000002E-2</v>
+        <v>0.11602899999999999</v>
       </c>
       <c r="D145">
-        <v>1300</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146">
-        <v>0.352771</v>
+        <v>0.52547900000000003</v>
       </c>
       <c r="B146">
-        <v>0.67614300000000005</v>
+        <v>0.214195</v>
       </c>
       <c r="C146">
-        <v>0.69501599999999997</v>
+        <v>0.845333</v>
       </c>
       <c r="D146">
-        <v>1270</v>
+        <v>522</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147">
-        <v>0.30952099999999999</v>
+        <v>0.52554199999999995</v>
       </c>
       <c r="B147">
-        <v>0.71531999999999996</v>
+        <v>8.1555500000000003E-2</v>
       </c>
       <c r="C147">
-        <v>0.11602899999999999</v>
+        <v>6.8555599999999994E-2</v>
       </c>
       <c r="D147">
-        <v>1215</v>
+        <v>386</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148">
-        <v>0.52547900000000003</v>
+        <v>0.17569000000000001</v>
       </c>
       <c r="B148">
-        <v>0.214195</v>
+        <v>0.189301</v>
       </c>
       <c r="C148">
-        <v>0.845333</v>
+        <v>0.76857600000000004</v>
       </c>
       <c r="D148">
-        <v>522</v>
+        <v>315</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149">
-        <v>0.52554199999999995</v>
+        <v>0.39589600000000003</v>
       </c>
       <c r="B149">
-        <v>8.1555500000000003E-2</v>
+        <v>0.50056500000000004</v>
       </c>
       <c r="C149">
-        <v>6.8555599999999994E-2</v>
+        <v>0.57168699999999995</v>
       </c>
       <c r="D149">
-        <v>386</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150">
-        <v>0.17569000000000001</v>
+        <v>0.14429800000000001</v>
       </c>
       <c r="B150">
-        <v>0.189301</v>
+        <v>0.68004399999999998</v>
       </c>
       <c r="C150">
-        <v>0.76857600000000004</v>
+        <v>3.2139800000000003E-2</v>
       </c>
       <c r="D150">
-        <v>315</v>
+        <v>996</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151">
-        <v>0.39589600000000003</v>
+        <v>0.42135699999999998</v>
       </c>
       <c r="B151">
-        <v>0.50056500000000004</v>
+        <v>0.10581599999999999</v>
       </c>
       <c r="C151">
-        <v>0.57168699999999995</v>
+        <v>0.85961900000000002</v>
       </c>
       <c r="D151">
-        <v>1070</v>
+        <v>312</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152">
-        <v>0.14429800000000001</v>
+        <v>0.37545400000000001</v>
       </c>
       <c r="B152">
-        <v>0.68004399999999998</v>
+        <v>3.9545300000000004E-3</v>
       </c>
       <c r="C152">
-        <v>3.2139800000000003E-2</v>
+        <v>1.8784699999999999E-3</v>
       </c>
       <c r="D152">
-        <v>996</v>
+        <v>183</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153">
-        <v>0.42135699999999998</v>
+        <v>0.40618900000000002</v>
       </c>
       <c r="B153">
-        <v>0.10581599999999999</v>
+        <v>0.52786299999999997</v>
       </c>
       <c r="C153">
-        <v>0.85961900000000002</v>
+        <v>0.57625599999999999</v>
       </c>
       <c r="D153">
-        <v>312</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154">
-        <v>0.37545400000000001</v>
+        <v>0.16224</v>
       </c>
       <c r="B154">
-        <v>3.9545300000000004E-3</v>
+        <v>0.70350800000000002</v>
       </c>
       <c r="C154">
-        <v>1.8784699999999999E-3</v>
+        <v>3.4238499999999998E-2</v>
       </c>
       <c r="D154">
-        <v>183</v>
+        <v>996</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155">
-        <v>0.40618900000000002</v>
+        <v>0.41200199999999998</v>
       </c>
       <c r="B155">
-        <v>0.52786299999999997</v>
+        <v>0.10148699999999999</v>
       </c>
       <c r="C155">
-        <v>0.57625599999999999</v>
+        <v>0.82403800000000005</v>
       </c>
       <c r="D155">
-        <v>1070</v>
+        <v>312</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156">
-        <v>0.16224</v>
+        <v>0.36166100000000001</v>
       </c>
       <c r="B156">
-        <v>0.70350800000000002</v>
+        <v>3.6154300000000002E-3</v>
       </c>
       <c r="C156">
-        <v>3.4238499999999998E-2</v>
+        <v>2.02688E-3</v>
       </c>
       <c r="D156">
-        <v>996</v>
+        <v>183</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157">
-        <v>0.41200199999999998</v>
+        <v>0.17857999999999999</v>
       </c>
       <c r="B157">
-        <v>0.10148699999999999</v>
+        <v>0.74829400000000001</v>
       </c>
       <c r="C157">
-        <v>0.82403800000000005</v>
+        <v>4.8257500000000002E-2</v>
       </c>
       <c r="D157">
-        <v>312</v>
+        <v>996</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158">
-        <v>0.36166100000000001</v>
+        <v>0.51043799999999995</v>
       </c>
       <c r="B158">
-        <v>3.6154300000000002E-3</v>
+        <v>0.14169899999999999</v>
       </c>
       <c r="C158">
-        <v>2.02688E-3</v>
+        <v>0.94797299999999995</v>
       </c>
       <c r="D158">
-        <v>183</v>
+        <v>312</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159">
-        <v>0.17857999999999999</v>
+        <v>0.50777000000000005</v>
       </c>
       <c r="B159">
-        <v>0.74829400000000001</v>
+        <v>5.3700500000000003E-3</v>
       </c>
       <c r="C159">
-        <v>4.8257500000000002E-2</v>
+        <v>3.0158899999999998E-3</v>
       </c>
       <c r="D159">
-        <v>996</v>
+        <v>183</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160">
-        <v>0.51043799999999995</v>
+        <v>0.41887999999999997</v>
       </c>
       <c r="B160">
-        <v>0.14169899999999999</v>
+        <v>0.51590199999999997</v>
       </c>
       <c r="C160">
-        <v>0.94797299999999995</v>
+        <v>0.59902999999999995</v>
       </c>
       <c r="D160">
-        <v>312</v>
+        <v>972</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161">
-        <v>0.50777000000000005</v>
+        <v>0.42520200000000002</v>
       </c>
       <c r="B161">
-        <v>5.3700500000000003E-3</v>
+        <v>0.52764</v>
       </c>
       <c r="C161">
-        <v>3.0158899999999998E-3</v>
+        <v>0.62226599999999999</v>
       </c>
       <c r="D161">
-        <v>183</v>
+        <v>963</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162">
-        <v>0.41887999999999997</v>
+        <v>0.40514699999999998</v>
       </c>
       <c r="B162">
-        <v>0.51590199999999997</v>
+        <v>0.49997999999999998</v>
       </c>
       <c r="C162">
-        <v>0.59902999999999995</v>
+        <v>0.61873</v>
       </c>
       <c r="D162">
-        <v>972</v>
+        <v>920</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163">
-        <v>0.42520200000000002</v>
+        <v>0.368979</v>
       </c>
       <c r="B163">
-        <v>0.52764</v>
+        <v>0.46040399999999998</v>
       </c>
       <c r="C163">
-        <v>0.62226599999999999</v>
+        <v>0.59051699999999996</v>
       </c>
       <c r="D163">
-        <v>963</v>
+        <v>840</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164">
-        <v>0.40514699999999998</v>
+        <v>0.33995799999999998</v>
       </c>
       <c r="B164">
-        <v>0.49997999999999998</v>
+        <v>0.424454</v>
       </c>
       <c r="C164">
-        <v>0.61873</v>
+        <v>0.55002600000000001</v>
       </c>
       <c r="D164">
-        <v>920</v>
+        <v>775</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165">
-        <v>0.368979</v>
+        <v>0.30617899999999998</v>
       </c>
       <c r="B165">
-        <v>0.46040399999999998</v>
+        <v>0.38794899999999999</v>
       </c>
       <c r="C165">
-        <v>0.59051699999999996</v>
+        <v>0.50526899999999997</v>
       </c>
       <c r="D165">
-        <v>840</v>
+        <v>690</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166">
-        <v>0.33995799999999998</v>
+        <v>0.26650299999999999</v>
       </c>
       <c r="B166">
-        <v>0.424454</v>
+        <v>0.35467700000000002</v>
       </c>
       <c r="C166">
-        <v>0.55002600000000001</v>
+        <v>0.461816</v>
       </c>
       <c r="D166">
-        <v>775</v>
+        <v>600</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167">
-        <v>0.30617899999999998</v>
+        <v>0.21376999999999999</v>
       </c>
       <c r="B167">
-        <v>0.38794899999999999</v>
+        <v>0.303672</v>
       </c>
       <c r="C167">
-        <v>0.50526899999999997</v>
+        <v>0.39129199999999997</v>
       </c>
       <c r="D167">
-        <v>690</v>
+        <v>500</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168">
-        <v>0.26650299999999999</v>
+        <v>0.159022</v>
       </c>
       <c r="B168">
-        <v>0.35467700000000002</v>
+        <v>0.23311100000000001</v>
       </c>
       <c r="C168">
-        <v>0.461816</v>
+        <v>0.31739899999999999</v>
       </c>
       <c r="D168">
-        <v>600</v>
+        <v>397</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169">
-        <v>0.21376999999999999</v>
+        <v>0.10792</v>
       </c>
       <c r="B169">
-        <v>0.303672</v>
+        <v>0.151362</v>
       </c>
       <c r="C169">
-        <v>0.39129199999999997</v>
+        <v>0.22768099999999999</v>
       </c>
       <c r="D169">
-        <v>500</v>
+        <v>298</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170">
-        <v>0.159022</v>
+        <v>5.7381000000000001E-2</v>
       </c>
       <c r="B170">
-        <v>0.23311100000000001</v>
+        <v>8.1146499999999996E-2</v>
       </c>
       <c r="C170">
-        <v>0.31739899999999999</v>
+        <v>0.119821</v>
       </c>
       <c r="D170">
-        <v>397</v>
+        <v>200</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171">
-        <v>0.10792</v>
+        <v>0.40416400000000002</v>
       </c>
       <c r="B171">
-        <v>0.151362</v>
+        <v>0.512629</v>
       </c>
       <c r="C171">
-        <v>0.22768099999999999</v>
+        <v>0.60165400000000002</v>
       </c>
       <c r="D171">
-        <v>298</v>
+        <v>972</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172">
-        <v>5.7381000000000001E-2</v>
+        <v>0.40462300000000001</v>
       </c>
       <c r="B172">
-        <v>8.1146499999999996E-2</v>
+        <v>0.50918699999999995</v>
       </c>
       <c r="C172">
-        <v>0.119821</v>
+        <v>0.615734</v>
       </c>
       <c r="D172">
-        <v>200</v>
+        <v>963</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173">
-        <v>0.40416400000000002</v>
+        <v>0.37877699999999997</v>
       </c>
       <c r="B173">
-        <v>0.512629</v>
+        <v>0.47750900000000002</v>
       </c>
       <c r="C173">
-        <v>0.60165400000000002</v>
+        <v>0.60387400000000002</v>
       </c>
       <c r="D173">
-        <v>972</v>
+        <v>920</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174">
-        <v>0.40462300000000001</v>
+        <v>0.34455000000000002</v>
       </c>
       <c r="B174">
-        <v>0.50918699999999995</v>
+        <v>0.43246800000000002</v>
       </c>
       <c r="C174">
-        <v>0.615734</v>
+        <v>0.56467699999999998</v>
       </c>
       <c r="D174">
-        <v>963</v>
+        <v>840</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175">
-        <v>0.37877699999999997</v>
+        <v>0.31514300000000001</v>
       </c>
       <c r="B175">
-        <v>0.47750900000000002</v>
+        <v>0.396032</v>
       </c>
       <c r="C175">
-        <v>0.60387400000000002</v>
+        <v>0.51902899999999996</v>
       </c>
       <c r="D175">
-        <v>920</v>
+        <v>775</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176">
-        <v>0.34455000000000002</v>
+        <v>0.27948899999999999</v>
       </c>
       <c r="B176">
-        <v>0.43246800000000002</v>
+        <v>0.35149000000000002</v>
       </c>
       <c r="C176">
-        <v>0.56467699999999998</v>
+        <v>0.46792299999999998</v>
       </c>
       <c r="D176">
-        <v>840</v>
+        <v>690</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177">
-        <v>0.31514300000000001</v>
+        <v>0.23527500000000001</v>
       </c>
       <c r="B177">
-        <v>0.396032</v>
+        <v>0.307257</v>
       </c>
       <c r="C177">
-        <v>0.51902899999999996</v>
+        <v>0.41327000000000003</v>
       </c>
       <c r="D177">
-        <v>775</v>
+        <v>600</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178">
-        <v>0.27948899999999999</v>
+        <v>0.18798599999999999</v>
       </c>
       <c r="B178">
-        <v>0.35149000000000002</v>
+        <v>0.25139800000000001</v>
       </c>
       <c r="C178">
-        <v>0.46792299999999998</v>
+        <v>0.34928599999999999</v>
       </c>
       <c r="D178">
-        <v>690</v>
+        <v>500</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179">
-        <v>0.23527500000000001</v>
+        <v>0.13964599999999999</v>
       </c>
       <c r="B179">
-        <v>0.307257</v>
+        <v>0.18728</v>
       </c>
       <c r="C179">
-        <v>0.41327000000000003</v>
+        <v>0.27098899999999998</v>
       </c>
       <c r="D179">
-        <v>600</v>
+        <v>397</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180">
-        <v>0.18798599999999999</v>
+        <v>0.24838099999999999</v>
       </c>
       <c r="B180">
-        <v>0.25139800000000001</v>
+        <v>0.32344600000000001</v>
       </c>
       <c r="C180">
-        <v>0.34928599999999999</v>
+        <v>0.40504200000000001</v>
       </c>
       <c r="D180">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181">
-        <v>0.13964599999999999</v>
+        <v>0.21255499999999999</v>
       </c>
       <c r="B181">
-        <v>0.18728</v>
+        <v>0.28800500000000001</v>
       </c>
       <c r="C181">
-        <v>0.27098899999999998</v>
+        <v>0.37623299999999998</v>
       </c>
       <c r="D181">
-        <v>397</v>
+        <v>500</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182">
-        <v>0.24838099999999999</v>
+        <v>0.17172799999999999</v>
       </c>
       <c r="B182">
-        <v>0.32344600000000001</v>
+        <v>0.24155299999999999</v>
       </c>
       <c r="C182">
-        <v>0.40504200000000001</v>
+        <v>0.32709899999999997</v>
       </c>
       <c r="D182">
-        <v>600</v>
+        <v>397</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183">
-        <v>0.21255499999999999</v>
+        <v>0.12895799999999999</v>
       </c>
       <c r="B183">
-        <v>0.28800500000000001</v>
+        <v>0.186362</v>
       </c>
       <c r="C183">
-        <v>0.37623299999999998</v>
+        <v>0.26326699999999997</v>
       </c>
       <c r="D183">
-        <v>500</v>
+        <v>298</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184">
-        <v>0.17172799999999999</v>
+        <v>8.7350200000000003E-2</v>
       </c>
       <c r="B184">
-        <v>0.24155299999999999</v>
+        <v>0.12540000000000001</v>
       </c>
       <c r="C184">
-        <v>0.32709899999999997</v>
+        <v>0.18684400000000001</v>
       </c>
       <c r="D184">
-        <v>397</v>
+        <v>200</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185">
-        <v>0.12895799999999999</v>
+        <v>0.365066</v>
       </c>
       <c r="B185">
-        <v>0.186362</v>
+        <v>0.46227099999999999</v>
       </c>
       <c r="C185">
-        <v>0.26326699999999997</v>
+        <v>0.52438399999999996</v>
       </c>
       <c r="D185">
-        <v>298</v>
+        <v>972</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186">
-        <v>8.7350200000000003E-2</v>
+        <v>0.37432700000000002</v>
       </c>
       <c r="B186">
-        <v>0.12540000000000001</v>
+        <v>0.48327700000000001</v>
       </c>
       <c r="C186">
-        <v>0.18684400000000001</v>
+        <v>0.55484599999999995</v>
       </c>
       <c r="D186">
-        <v>200</v>
+        <v>963</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187">
-        <v>0.365066</v>
+        <v>0.36328199999999999</v>
       </c>
       <c r="B187">
-        <v>0.46227099999999999</v>
+        <v>0.47761799999999999</v>
       </c>
       <c r="C187">
-        <v>0.52438399999999996</v>
+        <v>0.55093999999999999</v>
       </c>
       <c r="D187">
-        <v>972</v>
+        <v>920</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188">
-        <v>0.37432700000000002</v>
+        <v>0.33384000000000003</v>
       </c>
       <c r="B188">
-        <v>0.48327700000000001</v>
+        <v>0.44614700000000002</v>
       </c>
       <c r="C188">
-        <v>0.55484599999999995</v>
+        <v>0.52143600000000001</v>
       </c>
       <c r="D188">
-        <v>963</v>
+        <v>840</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189">
-        <v>0.36328199999999999</v>
+        <v>0.31409700000000002</v>
       </c>
       <c r="B189">
-        <v>0.47761799999999999</v>
+        <v>0.42398400000000003</v>
       </c>
       <c r="C189">
-        <v>0.55093999999999999</v>
+        <v>0.494479</v>
       </c>
       <c r="D189">
-        <v>920</v>
+        <v>775</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190">
-        <v>0.33384000000000003</v>
+        <v>0.28002899999999997</v>
       </c>
       <c r="B190">
-        <v>0.44614700000000002</v>
+        <v>0.387216</v>
       </c>
       <c r="C190">
-        <v>0.52143600000000001</v>
+        <v>0.45262200000000002</v>
       </c>
       <c r="D190">
-        <v>840</v>
+        <v>690</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191">
-        <v>0.31409700000000002</v>
+        <v>0.23855999999999999</v>
       </c>
       <c r="B191">
-        <v>0.42398400000000003</v>
+        <v>0.34304800000000002</v>
       </c>
       <c r="C191">
-        <v>0.494479</v>
+        <v>0.40309400000000001</v>
       </c>
       <c r="D191">
-        <v>775</v>
+        <v>600</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192">
-        <v>0.28002899999999997</v>
+        <v>0.19084000000000001</v>
       </c>
       <c r="B192">
-        <v>0.387216</v>
+        <v>0.287246</v>
       </c>
       <c r="C192">
-        <v>0.45262200000000002</v>
+        <v>0.34481899999999999</v>
       </c>
       <c r="D192">
-        <v>690</v>
+        <v>500</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193">
-        <v>0.23855999999999999</v>
+        <v>0.14114699999999999</v>
       </c>
       <c r="B193">
-        <v>0.34304800000000002</v>
+        <v>0.21953400000000001</v>
       </c>
       <c r="C193">
-        <v>0.40309400000000001</v>
+        <v>0.27692600000000001</v>
       </c>
       <c r="D193">
-        <v>600</v>
+        <v>397</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194">
-        <v>0.19084000000000001</v>
+        <v>9.7839099999999998E-2</v>
       </c>
       <c r="B194">
-        <v>0.287246</v>
+        <v>0.150284</v>
       </c>
       <c r="C194">
-        <v>0.34481899999999999</v>
+        <v>0.19386100000000001</v>
       </c>
       <c r="D194">
-        <v>500</v>
+        <v>298</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195">
-        <v>0.14114699999999999</v>
+        <v>5.1699599999999998E-2</v>
       </c>
       <c r="B195">
-        <v>0.21953400000000001</v>
+        <v>7.8857200000000002E-2</v>
       </c>
       <c r="C195">
-        <v>0.27692600000000001</v>
+        <v>9.9174399999999996E-2</v>
       </c>
       <c r="D195">
-        <v>397</v>
+        <v>200</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196">
-        <v>9.7839099999999998E-2</v>
+        <v>0.35117399999999999</v>
       </c>
       <c r="B196">
-        <v>0.150284</v>
+        <v>0.45335799999999998</v>
       </c>
       <c r="C196">
-        <v>0.19386100000000001</v>
+        <v>0.50822699999999998</v>
       </c>
       <c r="D196">
-        <v>298</v>
+        <v>920</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197">
-        <v>5.1699599999999998E-2</v>
+        <v>0.32609100000000002</v>
       </c>
       <c r="B197">
-        <v>7.8857200000000002E-2</v>
+        <v>0.42976700000000001</v>
       </c>
       <c r="C197">
-        <v>9.9174399999999996E-2</v>
+        <v>0.49113400000000001</v>
       </c>
       <c r="D197">
-        <v>200</v>
+        <v>840</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198">
-        <v>0.35117399999999999</v>
+        <v>0.30853799999999998</v>
       </c>
       <c r="B198">
-        <v>0.45335799999999998</v>
+        <v>0.41471200000000003</v>
       </c>
       <c r="C198">
-        <v>0.50822699999999998</v>
+        <v>0.47451700000000002</v>
       </c>
       <c r="D198">
-        <v>920</v>
+        <v>775</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199">
-        <v>0.32609100000000002</v>
+        <v>0.28128599999999998</v>
       </c>
       <c r="B199">
-        <v>0.42976700000000001</v>
+        <v>0.38482100000000002</v>
       </c>
       <c r="C199">
-        <v>0.49113400000000001</v>
+        <v>0.444471</v>
       </c>
       <c r="D199">
-        <v>840</v>
+        <v>690</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200">
-        <v>0.30853799999999998</v>
+        <v>0.24302099999999999</v>
       </c>
       <c r="B200">
-        <v>0.41471200000000003</v>
+        <v>0.34143099999999998</v>
       </c>
       <c r="C200">
-        <v>0.47451700000000002</v>
+        <v>0.396673</v>
       </c>
       <c r="D200">
-        <v>775</v>
+        <v>600</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201">
-        <v>0.28128599999999998</v>
+        <v>0.19475999999999999</v>
       </c>
       <c r="B201">
-        <v>0.38482100000000002</v>
+        <v>0.286165</v>
       </c>
       <c r="C201">
-        <v>0.444471</v>
+        <v>0.34456599999999998</v>
       </c>
       <c r="D201">
-        <v>690</v>
+        <v>500</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202">
-        <v>0.24302099999999999</v>
+        <v>0.14564299999999999</v>
       </c>
       <c r="B202">
-        <v>0.34143099999999998</v>
+        <v>0.22275600000000001</v>
       </c>
       <c r="C202">
-        <v>0.396673</v>
+        <v>0.28381800000000001</v>
       </c>
       <c r="D202">
-        <v>600</v>
+        <v>397</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203">
-        <v>0.19475999999999999</v>
+        <v>0.101546</v>
       </c>
       <c r="B203">
-        <v>0.286165</v>
+        <v>0.15867300000000001</v>
       </c>
       <c r="C203">
-        <v>0.34456599999999998</v>
+        <v>0.20191600000000001</v>
       </c>
       <c r="D203">
-        <v>500</v>
+        <v>298</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204">
-        <v>0.14564299999999999</v>
+        <v>5.5132E-2</v>
       </c>
       <c r="B204">
-        <v>0.22275600000000001</v>
+        <v>8.6966500000000002E-2</v>
       </c>
       <c r="C204">
-        <v>0.28381800000000001</v>
+        <v>0.106044</v>
       </c>
       <c r="D204">
-        <v>397</v>
+        <v>200</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205">
-        <v>0.101546</v>
+        <v>1.97419E-2</v>
       </c>
       <c r="B205">
-        <v>0.15867300000000001</v>
+        <v>2.8016300000000001E-2</v>
       </c>
       <c r="C205">
-        <v>0.20191600000000001</v>
+        <v>3.4755800000000003E-2</v>
       </c>
       <c r="D205">
-        <v>298</v>
+        <v>103</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206">
-        <v>5.5132E-2</v>
+        <v>2.3701E-2</v>
       </c>
       <c r="B206">
-        <v>8.6966500000000002E-2</v>
+        <v>3.05659E-2</v>
       </c>
       <c r="C206">
-        <v>0.106044</v>
-      </c>
-      <c r="D206">
-        <v>200</v>
+        <v>3.9891799999999998E-2</v>
+      </c>
+      <c r="D206" s="1">
+        <v>78</v>
+      </c>
+      <c r="E206" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207">
-        <v>1.97419E-2</v>
+        <v>5.2868100000000001E-2</v>
       </c>
       <c r="B207">
-        <v>2.8016300000000001E-2</v>
+        <v>6.7843299999999995E-2</v>
       </c>
       <c r="C207">
-        <v>3.4755800000000003E-2</v>
-      </c>
-      <c r="D207">
-        <v>103</v>
+        <v>8.7756399999999998E-2</v>
+      </c>
+      <c r="D207" s="1">
+        <v>231</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208">
-        <v>8.5971199999999998E-3</v>
+        <v>9.7904000000000005E-2</v>
       </c>
       <c r="B208">
-        <v>4.8982499999999998E-3</v>
+        <v>0.124985</v>
       </c>
       <c r="C208">
-        <v>2.3341799999999999E-3</v>
+        <v>0.16112599999999999</v>
       </c>
       <c r="D208" s="1">
-        <v>52</v>
-      </c>
-      <c r="E208" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209">
-        <v>2.3701E-2</v>
+        <v>2.9576400000000001E-3</v>
       </c>
       <c r="B209">
-        <v>3.05659E-2</v>
+        <v>2.2209300000000001E-2</v>
       </c>
       <c r="C209">
-        <v>3.9891799999999998E-2</v>
+        <v>6.3851300000000001E-3</v>
       </c>
       <c r="D209" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>7.1219199999999996E-2</v>
+      </c>
+      <c r="B210">
+        <v>6.2068900000000003E-2</v>
+      </c>
+      <c r="C210">
+        <v>3.7238599999999998E-3</v>
+      </c>
+      <c r="D210" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>2.8636999999999999E-2</v>
+      </c>
+      <c r="B211">
+        <v>4.2324700000000003E-3</v>
+      </c>
+      <c r="C211">
+        <v>2.41303E-2</v>
+      </c>
+      <c r="D211" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>1.7621399999999999E-3</v>
+      </c>
+      <c r="B212">
+        <v>2.04779E-2</v>
+      </c>
+      <c r="C212">
+        <v>4.4483300000000003E-2</v>
+      </c>
+      <c r="D212" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>6.4635200000000004E-2</v>
+      </c>
+      <c r="B213">
+        <v>2.4043399999999999E-2</v>
+      </c>
+      <c r="C213">
+        <v>2.6160200000000002E-3</v>
+      </c>
+      <c r="D213" s="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>1.9385599999999999E-2</v>
+      </c>
+      <c r="B214">
+        <v>5.3315300000000003E-2</v>
+      </c>
+      <c r="C214">
+        <v>5.7833299999999997E-3</v>
+      </c>
+      <c r="D214" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>3.1255499999999999E-2</v>
+      </c>
+      <c r="B215">
+        <v>3.6996799999999999E-3</v>
+      </c>
+      <c r="C215">
+        <v>6.5318399999999997E-3</v>
+      </c>
+      <c r="D215" s="1">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>4.4679400000000001E-2</v>
+      </c>
+      <c r="B216">
+        <v>7.4349799999999999E-3</v>
+      </c>
+      <c r="C216">
+        <v>1.32923E-3</v>
+      </c>
+      <c r="D216" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>3.5876900000000003E-2</v>
+      </c>
+      <c r="B217">
+        <v>2.26079E-2</v>
+      </c>
+      <c r="C217">
+        <v>2.2552300000000001E-2</v>
+      </c>
+      <c r="D217" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>5.6959799999999998E-3</v>
+      </c>
+      <c r="B218">
+        <v>1.2204E-2</v>
+      </c>
+      <c r="C218">
+        <v>3.34823E-2</v>
+      </c>
+      <c r="D218" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>1.30505E-2</v>
+      </c>
+      <c r="B219">
+        <v>1.4334899999999999E-2</v>
+      </c>
+      <c r="C219">
+        <v>4.88443E-2</v>
+      </c>
+      <c r="D219" s="1">
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>9.4468E-3</v>
+      </c>
+      <c r="B220">
+        <v>5.6413499999999998E-2</v>
+      </c>
+      <c r="C220">
+        <v>5.4308700000000001E-2</v>
+      </c>
+      <c r="D220" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>2.1636499999999999E-2</v>
+      </c>
+      <c r="B221">
+        <v>2.7144399999999999E-2</v>
+      </c>
+      <c r="C221">
+        <v>3.4917499999999997E-2</v>
+      </c>
+      <c r="D221" s="1">
         <v>78</v>
       </c>
-      <c r="E209" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A210">
-        <v>5.2868100000000001E-2</v>
-      </c>
-      <c r="B210">
-        <v>6.7843299999999995E-2</v>
-      </c>
-      <c r="C210">
-        <v>8.7756399999999998E-2</v>
-      </c>
-      <c r="D210" s="1">
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A222">
+        <v>4.84266E-2</v>
+      </c>
+      <c r="B222">
+        <v>6.0453399999999997E-2</v>
+      </c>
+      <c r="C222">
+        <v>7.7494599999999997E-2</v>
+      </c>
+      <c r="D222" s="1">
         <v>231</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A211">
-        <v>9.7904000000000005E-2</v>
-      </c>
-      <c r="B211">
-        <v>0.124985</v>
-      </c>
-      <c r="C211">
-        <v>0.16112599999999999</v>
-      </c>
-      <c r="D211" s="1">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A223">
+        <v>9.2013399999999995E-2</v>
+      </c>
+      <c r="B223">
+        <v>0.114135</v>
+      </c>
+      <c r="C223">
+        <v>0.14504500000000001</v>
+      </c>
+      <c r="D223" s="1">
         <v>355</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A212">
-        <v>2.2047899999999999E-3</v>
-      </c>
-      <c r="B212">
-        <v>2.7542000000000001E-3</v>
-      </c>
-      <c r="C212">
-        <v>2.4131699999999999E-2</v>
-      </c>
-      <c r="D212" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A213">
-        <v>2.9576400000000001E-3</v>
-      </c>
-      <c r="B213">
-        <v>2.2209300000000001E-2</v>
-      </c>
-      <c r="C213">
-        <v>6.3851300000000001E-3</v>
-      </c>
-      <c r="D213" s="1">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A224">
+        <v>2.8321100000000001E-3</v>
+      </c>
+      <c r="B224">
+        <v>1.9775500000000001E-2</v>
+      </c>
+      <c r="C224">
+        <v>5.6569200000000002E-3</v>
+      </c>
+      <c r="D224" s="1">
         <v>97</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A214">
-        <v>2.3538E-2</v>
-      </c>
-      <c r="B214">
-        <v>1.1210199999999999E-3</v>
-      </c>
-      <c r="C214">
-        <v>1.7938100000000001E-3</v>
-      </c>
-      <c r="D214" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A215">
-        <v>7.1219199999999996E-2</v>
-      </c>
-      <c r="B215">
-        <v>6.2068900000000003E-2</v>
-      </c>
-      <c r="C215">
-        <v>3.7238599999999998E-3</v>
-      </c>
-      <c r="D215" s="1">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A216">
-        <v>2.8636999999999999E-2</v>
-      </c>
-      <c r="B216">
-        <v>4.2324700000000003E-3</v>
-      </c>
-      <c r="C216">
-        <v>2.41303E-2</v>
-      </c>
-      <c r="D216" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A217">
-        <v>1.7621399999999999E-3</v>
-      </c>
-      <c r="B217">
-        <v>2.04779E-2</v>
-      </c>
-      <c r="C217">
-        <v>4.4483300000000003E-2</v>
-      </c>
-      <c r="D217" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A218">
-        <v>6.4635200000000004E-2</v>
-      </c>
-      <c r="B218">
-        <v>2.4043399999999999E-2</v>
-      </c>
-      <c r="C218">
-        <v>2.6160200000000002E-3</v>
-      </c>
-      <c r="D218" s="1">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A219">
-        <v>1.9385599999999999E-2</v>
-      </c>
-      <c r="B219">
-        <v>5.3315300000000003E-2</v>
-      </c>
-      <c r="C219">
-        <v>5.7833299999999997E-3</v>
-      </c>
-      <c r="D219" s="1">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A220">
-        <v>4.15498E-3</v>
-      </c>
-      <c r="B220">
-        <v>2.0171999999999998E-3</v>
-      </c>
-      <c r="C220">
-        <v>9.2993699999999995E-3</v>
-      </c>
-      <c r="D220" s="1">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A221">
-        <v>3.1255499999999999E-2</v>
-      </c>
-      <c r="B221">
-        <v>3.6996799999999999E-3</v>
-      </c>
-      <c r="C221">
-        <v>6.5318399999999997E-3</v>
-      </c>
-      <c r="D221" s="1">
-        <v>70.3</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A222">
-        <v>3.6369000000000002E-3</v>
-      </c>
-      <c r="B222">
-        <v>5.4739799999999998E-3</v>
-      </c>
-      <c r="C222">
-        <v>3.5549400000000002E-2</v>
-      </c>
-      <c r="D222" s="1">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A223">
-        <v>4.4679400000000001E-2</v>
-      </c>
-      <c r="B223">
-        <v>7.4349799999999999E-3</v>
-      </c>
-      <c r="C223">
-        <v>1.32923E-3</v>
-      </c>
-      <c r="D223" s="1">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A224">
-        <v>5.06544E-3</v>
-      </c>
-      <c r="B224">
-        <v>2.8142200000000001E-3</v>
-      </c>
-      <c r="C224">
-        <v>2.43706E-3</v>
-      </c>
-      <c r="D224" s="1">
-        <v>35</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225">
-        <v>3.5876900000000003E-2</v>
+        <v>6.72566E-2</v>
       </c>
       <c r="B225">
-        <v>2.26079E-2</v>
+        <v>5.6219999999999999E-2</v>
       </c>
       <c r="C225">
-        <v>2.2552300000000001E-2</v>
+        <v>3.4998099999999999E-3</v>
       </c>
       <c r="D225" s="1">
-        <v>130</v>
+        <v>250</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226">
-        <v>5.6959799999999998E-3</v>
+        <v>2.6381700000000001E-2</v>
       </c>
       <c r="B226">
-        <v>1.2204E-2</v>
+        <v>3.9327199999999998E-3</v>
       </c>
       <c r="C226">
-        <v>3.34823E-2</v>
+        <v>2.15371E-2</v>
       </c>
       <c r="D226" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227">
-        <v>2.9004299999999998E-3</v>
+        <v>1.7120499999999999E-3</v>
       </c>
       <c r="B227">
-        <v>5.6703500000000002E-3</v>
+        <v>1.8289699999999999E-2</v>
       </c>
       <c r="C227">
-        <v>2.6778399999999999E-3</v>
+        <v>3.9763600000000003E-2</v>
       </c>
       <c r="D227" s="1">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228">
-        <v>1.30505E-2</v>
+        <v>5.8779499999999998E-2</v>
       </c>
       <c r="B228">
-        <v>1.4334899999999999E-2</v>
+        <v>2.2137400000000002E-2</v>
       </c>
       <c r="C228">
-        <v>4.88443E-2</v>
+        <v>2.3088000000000002E-3</v>
       </c>
       <c r="D228" s="1">
-        <v>83.3</v>
+        <v>177</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229">
-        <v>9.4468E-3</v>
+        <v>1.8159999999999999E-2</v>
       </c>
       <c r="B229">
-        <v>5.6413499999999998E-2</v>
+        <v>4.7862599999999998E-2</v>
       </c>
       <c r="C229">
-        <v>5.4308700000000001E-2</v>
+        <v>5.4136200000000001E-3</v>
       </c>
       <c r="D229" s="1">
-        <v>153</v>
+        <v>183</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230">
-        <v>2.1636499999999999E-2</v>
+        <v>2.8906600000000001E-2</v>
       </c>
       <c r="B230">
-        <v>2.7144399999999999E-2</v>
+        <v>3.4510000000000001E-3</v>
       </c>
       <c r="C230">
-        <v>3.4917499999999997E-2</v>
+        <v>5.8234100000000002E-3</v>
       </c>
       <c r="D230" s="1">
-        <v>78</v>
+        <v>70.3</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231">
-        <v>4.84266E-2</v>
+        <v>4.1082599999999997E-2</v>
       </c>
       <c r="B231">
-        <v>6.0453399999999997E-2</v>
+        <v>6.8660500000000003E-3</v>
       </c>
       <c r="C231">
-        <v>7.7494599999999997E-2</v>
+        <v>1.2752900000000001E-3</v>
       </c>
       <c r="D231" s="1">
-        <v>231</v>
+        <v>102</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232">
-        <v>9.2013399999999995E-2</v>
+        <v>3.2911700000000002E-2</v>
       </c>
       <c r="B232">
-        <v>0.114135</v>
+        <v>2.0512699999999998E-2</v>
       </c>
       <c r="C232">
-        <v>0.14504500000000001</v>
+        <v>2.0257899999999999E-2</v>
       </c>
       <c r="D232" s="1">
-        <v>355</v>
+        <v>130</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233">
-        <v>2.1565500000000001E-3</v>
+        <v>5.1622899999999999E-3</v>
       </c>
       <c r="B233">
-        <v>2.4702000000000001E-3</v>
+        <v>1.10262E-2</v>
       </c>
       <c r="C233">
-        <v>2.19087E-2</v>
+        <v>2.9814500000000001E-2</v>
       </c>
       <c r="D233" s="1">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234">
-        <v>2.8321100000000001E-3</v>
+        <v>1.1668400000000001E-2</v>
       </c>
       <c r="B234">
-        <v>1.9775500000000001E-2</v>
+        <v>1.29295E-2</v>
       </c>
       <c r="C234">
-        <v>5.6569200000000002E-3</v>
+        <v>4.3041299999999998E-2</v>
       </c>
       <c r="D234" s="1">
-        <v>97</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235">
-        <v>2.1475299999999999E-2</v>
+        <v>8.73203E-3</v>
       </c>
       <c r="B235">
-        <v>1.0560599999999999E-3</v>
+        <v>5.06454E-2</v>
       </c>
       <c r="C235">
-        <v>1.7290199999999999E-3</v>
+        <v>4.8091700000000001E-2</v>
       </c>
       <c r="D235" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A236">
-        <v>6.72566E-2</v>
-      </c>
-      <c r="B236">
-        <v>5.6219999999999999E-2</v>
-      </c>
-      <c r="C236">
-        <v>3.4998099999999999E-3</v>
-      </c>
-      <c r="D236" s="1">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A237">
-        <v>2.6381700000000001E-2</v>
-      </c>
-      <c r="B237">
-        <v>3.9327199999999998E-3</v>
-      </c>
-      <c r="C237">
-        <v>2.15371E-2</v>
-      </c>
-      <c r="D237" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A238">
-        <v>1.7120499999999999E-3</v>
-      </c>
-      <c r="B238">
-        <v>1.8289699999999999E-2</v>
-      </c>
-      <c r="C238">
-        <v>3.9763600000000003E-2</v>
-      </c>
-      <c r="D238" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A239">
-        <v>5.8779499999999998E-2</v>
-      </c>
-      <c r="B239">
-        <v>2.2137400000000002E-2</v>
-      </c>
-      <c r="C239">
-        <v>2.3088000000000002E-3</v>
-      </c>
-      <c r="D239" s="1">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A240">
-        <v>1.8159999999999999E-2</v>
-      </c>
-      <c r="B240">
-        <v>4.7862599999999998E-2</v>
-      </c>
-      <c r="C240">
-        <v>5.4136200000000001E-3</v>
-      </c>
-      <c r="D240" s="1">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A241">
-        <v>3.7201299999999999E-3</v>
-      </c>
-      <c r="B241">
-        <v>1.93721E-3</v>
-      </c>
-      <c r="C241">
-        <v>8.22758E-3</v>
-      </c>
-      <c r="D241" s="1">
-        <v>25.7</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A242">
-        <v>2.8906600000000001E-2</v>
-      </c>
-      <c r="B242">
-        <v>3.4510000000000001E-3</v>
-      </c>
-      <c r="C242">
-        <v>5.8234100000000002E-3</v>
-      </c>
-      <c r="D242" s="1">
-        <v>70.3</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A243">
-        <v>3.3527600000000002E-3</v>
-      </c>
-      <c r="B243">
-        <v>4.9668999999999998E-3</v>
-      </c>
-      <c r="C243">
-        <v>3.1616900000000003E-2</v>
-      </c>
-      <c r="D243" s="1">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A244">
-        <v>4.1082599999999997E-2</v>
-      </c>
-      <c r="B244">
-        <v>6.8660500000000003E-3</v>
-      </c>
-      <c r="C244">
-        <v>1.2752900000000001E-3</v>
-      </c>
-      <c r="D244" s="1">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A245">
-        <v>4.7777499999999999E-3</v>
-      </c>
-      <c r="B245">
-        <v>2.6144900000000001E-3</v>
-      </c>
-      <c r="C245">
-        <v>2.3516399999999999E-3</v>
-      </c>
-      <c r="D245" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A246">
-        <v>3.2911700000000002E-2</v>
-      </c>
-      <c r="B246">
-        <v>2.0512699999999998E-2</v>
-      </c>
-      <c r="C246">
-        <v>2.0257899999999999E-2</v>
-      </c>
-      <c r="D246" s="1">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A247">
-        <v>5.1622899999999999E-3</v>
-      </c>
-      <c r="B247">
-        <v>1.10262E-2</v>
-      </c>
-      <c r="C247">
-        <v>2.9814500000000001E-2</v>
-      </c>
-      <c r="D247" s="1">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A248">
-        <v>2.7393500000000002E-3</v>
-      </c>
-      <c r="B248">
-        <v>5.3840700000000003E-3</v>
-      </c>
-      <c r="C248">
-        <v>2.48511E-3</v>
-      </c>
-      <c r="D248" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A249">
-        <v>1.1668400000000001E-2</v>
-      </c>
-      <c r="B249">
-        <v>1.29295E-2</v>
-      </c>
-      <c r="C249">
-        <v>4.3041299999999998E-2</v>
-      </c>
-      <c r="D249" s="1">
-        <v>83.3</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A250">
-        <v>8.73203E-3</v>
-      </c>
-      <c r="B250">
-        <v>5.06454E-2</v>
-      </c>
-      <c r="C250">
-        <v>4.8091700000000001E-2</v>
-      </c>
-      <c r="D250" s="1">
         <v>153</v>
       </c>
     </row>

</xml_diff>